<commit_message>
Adding raw data for Georgia and Virginia and making some adjustments to the analysis.
</commit_message>
<xml_diff>
--- a/Data/Raw Data/Georgia_CO2.xlsx
+++ b/Data/Raw Data/Georgia_CO2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7926cc0037b1217d/Documents/MIDP/SS/R/Team Group/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{3529A2AF-8C47-4658-B259-E7B35B63443D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96E02522-6117-4144-957B-2AA046EF039C}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{3529A2AF-8C47-4658-B259-E7B35B63443D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{576276FE-704C-4A27-ADBE-8C47E837E437}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{19A0FEA3-ED56-4D8E-A3BA-4AF8B4051AB3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
   <si>
     <t>million metric tons of CO2</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Georgia Carbon Dioxide Emissions from Fossil Fuel Consumption (1970-2021)</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -209,6 +215,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,7 +521,7 @@
   <dimension ref="A1:BB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,8 +543,12 @@
       </c>
     </row>
     <row r="4" spans="1:54" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="4">
         <v>1970</v>
       </c>

</xml_diff>